<commit_message>
Actualización y re-estructuración del código
</commit_message>
<xml_diff>
--- a/Descriptivos/Estadisticas_Agrupadas_Sin_Extremos.xlsx
+++ b/Descriptivos/Estadisticas_Agrupadas_Sin_Extremos.xlsx
@@ -38,55 +38,55 @@
     <t xml:space="preserve">max</t>
   </si>
   <si>
-    <t xml:space="preserve">goldEarned.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kills.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deaths.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assists.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">champExperience.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">player.WR.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">turretKills.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totalMinionsKilled.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totalTimeCCDealt.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baronKills.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dragonKills.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totalDamageDealt.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totalDamageTaken.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totalDamageDealtToChampions.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">damageDealtToObjectives.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goldEarnedPerMinute.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visionScore.mean</t>
+    <t xml:space="preserve">goldEarned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">champExperience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">player.WR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turretKills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalMinionsKilled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalTimeCCDealt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baronKills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dragonKills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalDamageDealt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalDamageTaken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalDamageDealtToChampions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">damageDealtToObjectives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goldEarnedPerMinute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visionScore</t>
   </si>
 </sst>
 </file>
@@ -449,25 +449,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>10441.4786908664</v>
+        <v>10382.1815339248</v>
       </c>
       <c r="C2" t="n">
-        <v>1889.17560404714</v>
+        <v>3852.53681543654</v>
       </c>
       <c r="D2" t="n">
-        <v>5819</v>
+        <v>500</v>
       </c>
       <c r="E2" t="n">
-        <v>9843.53947368421</v>
+        <v>7544</v>
       </c>
       <c r="F2" t="n">
-        <v>10854.8333333333</v>
+        <v>9997</v>
       </c>
       <c r="G2" t="n">
-        <v>11583.6941176471</v>
+        <v>12896</v>
       </c>
       <c r="H2" t="n">
-        <v>21488.5</v>
+        <v>34146</v>
       </c>
     </row>
     <row r="3">
@@ -475,25 +475,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>5.40750624392466</v>
+        <v>5.28342273177924</v>
       </c>
       <c r="C3" t="n">
-        <v>2.18661605972566</v>
+        <v>4.32393789092404</v>
       </c>
       <c r="D3" t="n">
-        <v>0.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>4.20430107526882</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>5.78947368421053</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>6.8469387755102</v>
+        <v>8</v>
       </c>
       <c r="H3" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -501,25 +501,25 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>4.74610005196471</v>
+        <v>4.68032641024989</v>
       </c>
       <c r="C4" t="n">
-        <v>0.956225870237017</v>
+        <v>2.88871937527078</v>
       </c>
       <c r="D4" t="n">
-        <v>2.36363636363636</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>4.12941176470588</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>4.68674698795181</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>5.27659574468085</v>
+        <v>7</v>
       </c>
       <c r="H4" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -527,25 +527,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>7.79605943752964</v>
+        <v>7.78218979586649</v>
       </c>
       <c r="C5" t="n">
-        <v>3.07904318575147</v>
+        <v>5.86532339793899</v>
       </c>
       <c r="D5" t="n">
-        <v>2.77777777777778</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>5.77894736842105</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>6.75</v>
+        <v>7</v>
       </c>
       <c r="G5" t="n">
-        <v>8.68</v>
+        <v>11</v>
       </c>
       <c r="H5" t="n">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6">
@@ -553,25 +553,25 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>11430.2330179044</v>
+        <v>11376.2405623205</v>
       </c>
       <c r="C6" t="n">
-        <v>1911.51837927268</v>
+        <v>4295.2504418734</v>
       </c>
       <c r="D6" t="n">
-        <v>5807.5</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>10348.2625</v>
+        <v>8228</v>
       </c>
       <c r="F6" t="n">
-        <v>11679.8333333333</v>
+        <v>11205</v>
       </c>
       <c r="G6" t="n">
-        <v>12795.8977272727</v>
+        <v>14214</v>
       </c>
       <c r="H6" t="n">
-        <v>21603.5</v>
+        <v>33483</v>
       </c>
     </row>
     <row r="7">
@@ -579,22 +579,22 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>0.538432993519736</v>
+        <v>0.538627755039784</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0792972499346495</v>
+        <v>0.0651390355652344</v>
       </c>
       <c r="D7" t="n">
         <v>0.285714285714286</v>
       </c>
       <c r="E7" t="n">
-        <v>0.49438202247191</v>
+        <v>0.494623655913978</v>
       </c>
       <c r="F7" t="n">
-        <v>0.534883720930233</v>
+        <v>0.536842105263158</v>
       </c>
       <c r="G7" t="n">
-        <v>0.581395348837209</v>
+        <v>0.578313253012048</v>
       </c>
       <c r="H7" t="n">
         <v>0.863636363636364</v>
@@ -605,25 +605,25 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>1.06979827579464</v>
+        <v>1.07204413147927</v>
       </c>
       <c r="C8" t="n">
-        <v>0.641317299923443</v>
+        <v>1.38759051478975</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.583333333333333</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1.09677419354839</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>1.51162790697674</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -631,25 +631,25 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>119.221756056726</v>
+        <v>119.788545135623</v>
       </c>
       <c r="C9" t="n">
-        <v>79.9651434783293</v>
+        <v>89.7849912242387</v>
       </c>
       <c r="D9" t="n">
-        <v>14.6551724137931</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" t="n">
-        <v>171.116279069767</v>
+        <v>132</v>
       </c>
       <c r="G9" t="n">
-        <v>188.663043478261</v>
+        <v>195</v>
       </c>
       <c r="H9" t="n">
-        <v>248</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10">
@@ -657,25 +657,25 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>243.45862042091</v>
+        <v>243.634745913517</v>
       </c>
       <c r="C10" t="n">
-        <v>142.217697170663</v>
+        <v>353.129174670099</v>
       </c>
       <c r="D10" t="n">
-        <v>68.4285714285714</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>147.785714285714</v>
+        <v>80</v>
       </c>
       <c r="F10" t="n">
-        <v>196.214285714286</v>
+        <v>161</v>
       </c>
       <c r="G10" t="n">
-        <v>307.053191489362</v>
+        <v>288</v>
       </c>
       <c r="H10" t="n">
-        <v>1303.375</v>
+        <v>6151</v>
       </c>
     </row>
     <row r="11">
@@ -683,25 +683,25 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>0.102258687891308</v>
+        <v>0.102270127361009</v>
       </c>
       <c r="C11" t="n">
-        <v>0.147639707911504</v>
+        <v>0.335723354528011</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0105263157894737</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0319148936170213</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.102272727272727</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0.75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -709,25 +709,25 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>0.31531102470189</v>
+        <v>0.316445077153825</v>
       </c>
       <c r="C12" t="n">
-        <v>0.50769510753627</v>
+        <v>0.737393054875219</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0158730158730159</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0537634408602151</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.208333333333333</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -735,25 +735,25 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>122417.774604168</v>
+        <v>121562.940361492</v>
       </c>
       <c r="C13" t="n">
-        <v>55460.3651950468</v>
+        <v>81143.5594554608</v>
       </c>
       <c r="D13" t="n">
-        <v>14769.5714285714</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>113047.82278481</v>
+        <v>57244</v>
       </c>
       <c r="F13" t="n">
-        <v>135488.483870968</v>
+        <v>115956</v>
       </c>
       <c r="G13" t="n">
-        <v>158606.966666667</v>
+        <v>172198</v>
       </c>
       <c r="H13" t="n">
-        <v>273354</v>
+        <v>639246</v>
       </c>
     </row>
     <row r="14">
@@ -761,25 +761,25 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>20232.5500743418</v>
+        <v>20014.8134834888</v>
       </c>
       <c r="C14" t="n">
-        <v>5020.43582492329</v>
+        <v>10341.2142431826</v>
       </c>
       <c r="D14" t="n">
-        <v>10669.9032258065</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>16217.3333333333</v>
+        <v>12494</v>
       </c>
       <c r="F14" t="n">
-        <v>19327.2653061224</v>
+        <v>18396</v>
       </c>
       <c r="G14" t="n">
-        <v>24213.835443038</v>
+        <v>25772</v>
       </c>
       <c r="H14" t="n">
-        <v>50133.3333333333</v>
+        <v>136330</v>
       </c>
     </row>
     <row r="15">
@@ -787,25 +787,25 @@
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>16833.3980412679</v>
+        <v>16520.6634466279</v>
       </c>
       <c r="C15" t="n">
-        <v>5814.10381366821</v>
+        <v>11066.9406952063</v>
       </c>
       <c r="D15" t="n">
-        <v>4974.20408163265</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>14126.6164383562</v>
+        <v>8140</v>
       </c>
       <c r="F15" t="n">
-        <v>17828.3626373626</v>
+        <v>14122</v>
       </c>
       <c r="G15" t="n">
-        <v>20350.140625</v>
+        <v>22353</v>
       </c>
       <c r="H15" t="n">
-        <v>53851</v>
+        <v>117333</v>
       </c>
     </row>
     <row r="16">
@@ -813,25 +813,25 @@
         <v>22</v>
       </c>
       <c r="B16" t="n">
-        <v>10802.2363232087</v>
+        <v>10770.8425909449</v>
       </c>
       <c r="C16" t="n">
-        <v>8479.30734459703</v>
+        <v>12394.2069318237</v>
       </c>
       <c r="D16" t="n">
-        <v>131.666666666667</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>4945.28571428571</v>
+        <v>1894</v>
       </c>
       <c r="F16" t="n">
-        <v>7827.82926829268</v>
+        <v>5949</v>
       </c>
       <c r="G16" t="n">
-        <v>13692.1666666667</v>
+        <v>15392</v>
       </c>
       <c r="H16" t="n">
-        <v>35216.2727272727</v>
+        <v>99712</v>
       </c>
     </row>
     <row r="17">
@@ -839,25 +839,25 @@
         <v>23</v>
       </c>
       <c r="B17" t="n">
-        <v>418.98863763899</v>
+        <v>418.080040864473</v>
       </c>
       <c r="C17" t="n">
-        <v>68.2745387945417</v>
+        <v>103.232457931167</v>
       </c>
       <c r="D17" t="n">
-        <v>266.553476605039</v>
+        <v>177.410071942446</v>
       </c>
       <c r="E17" t="n">
-        <v>405.400458717443</v>
+        <v>341.941747572816</v>
       </c>
       <c r="F17" t="n">
-        <v>438.191568618349</v>
+        <v>415.930949445129</v>
       </c>
       <c r="G17" t="n">
-        <v>462.281736172576</v>
+        <v>486.714801444043</v>
       </c>
       <c r="H17" t="n">
-        <v>615.53717240843</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="18">
@@ -865,25 +865,25 @@
         <v>24</v>
       </c>
       <c r="B18" t="n">
-        <v>30.5123674167521</v>
+        <v>30.5680911101507</v>
       </c>
       <c r="C18" t="n">
-        <v>16.8678330872343</v>
+        <v>23.1021717229153</v>
       </c>
       <c r="D18" t="n">
-        <v>8.525</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>19.9268292682927</v>
+        <v>16</v>
       </c>
       <c r="F18" t="n">
-        <v>23.5945945945946</v>
+        <v>24</v>
       </c>
       <c r="G18" t="n">
-        <v>31.0327868852459</v>
+        <v>37</v>
       </c>
       <c r="H18" t="n">
-        <v>96.25</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>